<commit_message>
change Real test tweets
</commit_message>
<xml_diff>
--- a/Dataset/RealTest.xlsx
+++ b/Dataset/RealTest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>There remains one person receiving hospital-level care for COVID-19; they are in Middlemore and are not in ICU. ⁣ ⁣ Yesterday our laboratories completed 2163 tests bringing the total number of tests completed to date to 261315. #COVID19nz #covid19</t>
   </si>
@@ -119,15 +119,6 @@
   </si>
   <si>
     <t>It has been 93 days since the last case of COVID-19 was acquired locally from an unknown source. The total number of active cases of COVID-19 in New Zealand’s managed isolation and quarantine facilities is now 25.</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>tweet</t>
-  </si>
-  <si>
-    <t>label</t>
   </si>
 </sst>
 </file>
@@ -476,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,22 +478,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
+      <c r="A1" s="1">
+        <v>6392</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>6388</v>
+        <v>6396</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -510,21 +501,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>6389</v>
+        <v>6393</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>6390</v>
+        <v>6391</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -532,32 +523,32 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>6391</v>
+        <v>6394</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>6392</v>
+        <v>6390</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6393</v>
+        <v>6395</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -565,21 +556,21 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6394</v>
+        <v>6389</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>6395</v>
+        <v>6397</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
@@ -587,10 +578,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>6396</v>
+        <v>6388</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
@@ -598,10 +589,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>6397</v>
+        <v>6398</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
@@ -609,46 +600,46 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>6398</v>
+        <v>6399</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>6399</v>
+        <v>6400</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>6400</v>
+        <v>6401</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>6401</v>
+        <v>6407</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,21 +655,21 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>6403</v>
+        <v>6408</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>6404</v>
+        <v>6403</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>1</v>
@@ -686,21 +677,21 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>6405</v>
+        <v>6409</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>6406</v>
+        <v>6404</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>1</v>
@@ -708,10 +699,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>6407</v>
+        <v>6410</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
@@ -719,21 +710,21 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>6408</v>
+        <v>6405</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>6409</v>
+        <v>6411</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
@@ -741,21 +732,21 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>6410</v>
+        <v>6406</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>6411</v>
+        <v>6413</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
@@ -772,12 +763,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>6413</v>
+        <v>6414</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
@@ -785,43 +776,43 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>6414</v>
+        <v>6415</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>6415</v>
+        <v>6416</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>6416</v>
+        <v>6417</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>6417</v>
+        <v>6418</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -829,10 +820,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>6418</v>
+        <v>6419</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
@@ -840,25 +831,19 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>6419</v>
+        <v>6420</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>6420</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>